<commit_message>
Fix excel axis labels
</commit_message>
<xml_diff>
--- a/excel/cars-sample.xlsx
+++ b/excel/cars-sample.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper\Documents\Classes\CS573 Data Visualization\a2-DataVis-5ways\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{389E84FC-BB1C-4BB0-8D32-7DC03DE50208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A7DD44-EADB-4753-8C7A-BE454C02420E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cars-sample.excel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -286,7 +298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5472,6 +5484,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Weight</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -5538,6 +5605,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>MPG</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -6280,8 +6402,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B1:P98" totalsRowShown="0">
-  <autoFilter ref="B1:P98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B1:P98" totalsRowShown="0">
+  <autoFilter ref="B1:P98" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="10"/>
@@ -6345,29 +6467,29 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" name="Car"/>
-    <tableColumn id="2" name="Manufacturer"/>
-    <tableColumn id="3" name="MPG"/>
-    <tableColumn id="4" name="Cylinders"/>
-    <tableColumn id="5" name="Displacement"/>
-    <tableColumn id="6" name="Horsepower"/>
-    <tableColumn id="7" name="Weight"/>
-    <tableColumn id="8" name="Acceleration"/>
-    <tableColumn id="9" name="Model.Year"/>
-    <tableColumn id="10" name="Origin"/>
-    <tableColumn id="11" name="ford" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Car"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="MPG"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cylinders"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Displacement"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Horsepower"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Weight"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Acceleration"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Model.Year"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Origin"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ford" dataDxfId="4">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Manufacturer]]="ford",Table2[[#This Row],[MPG]], NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="toyota" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="toyota" dataDxfId="3">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Manufacturer]]="toyota",Table2[[#This Row],[MPG]], NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="bmw" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="bmw" dataDxfId="2">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Manufacturer]]="bmw",Table2[[#This Row],[MPG]], NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="honda" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="honda" dataDxfId="1">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Manufacturer]]="honda",Table2[[#This Row],[MPG]], NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="mercades" dataDxfId="4">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="mercades" dataDxfId="0">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Manufacturer]]="mercedes",Table2[[#This Row],[MPG]], NA())</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6671,11 +6793,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K9" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>